<commit_message>
Added MAC address data collection
</commit_message>
<xml_diff>
--- a/727-4251 DataSheet.xlsx
+++ b/727-4251 DataSheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dain\Documents\Github\MIS-4251_Functional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA06EA32-2D82-4B73-9DDA-ECA13B1CB328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A73E84-9B8B-4A7B-B36B-7202EE723CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{559B6F92-2AB9-4868-ADA8-841517E47FEB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{559B6F92-2AB9-4868-ADA8-841517E47FEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>727-4251 Final Test Report (05-10-08-022 Rev B)</t>
   </si>
@@ -249,6 +250,18 @@
   </si>
   <si>
     <t>Wifi MAC:</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -540,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -651,6 +664,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -662,30 +714,60 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -695,29 +777,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -726,81 +785,29 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1161,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11159E69-3848-4F90-98C6-74C554ACDCB0}">
   <dimension ref="A1:R92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:K4"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1188,20 +1195,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
+      <c r="B1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
       <c r="O1"/>
       <c r="P1" s="2" t="s">
         <v>1</v>
@@ -1225,17 +1232,17 @@
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="4"/>
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
@@ -1243,17 +1250,17 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
       <c r="H4" s="4"/>
       <c r="I4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
@@ -1261,70 +1268,70 @@
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="5"/>
       <c r="I5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="84"/>
-      <c r="K5" s="49"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="46"/>
       <c r="L5" s="3"/>
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="82"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="84"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="83"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="44"/>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
       <c r="M7" s="6"/>
       <c r="N7" s="1"/>
       <c r="O7"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="70" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="72"/>
+      <c r="J8" s="49"/>
       <c r="K8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1342,16 +1349,16 @@
       <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="11"/>
@@ -1363,16 +1370,16 @@
       <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="42"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="54"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="14" t="str">
@@ -1398,8 +1405,8 @@
       <c r="F11" s="57"/>
       <c r="G11" s="57"/>
       <c r="H11" s="57"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="54"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="14" t="str">
@@ -1425,8 +1432,8 @@
       <c r="F12" s="57"/>
       <c r="G12" s="57"/>
       <c r="H12" s="57"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="42"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="54"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="14" t="str">
@@ -1452,8 +1459,8 @@
       <c r="F13" s="57"/>
       <c r="G13" s="57"/>
       <c r="H13" s="57"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="42"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="14" t="str">
@@ -1479,8 +1486,8 @@
       <c r="F14" s="57"/>
       <c r="G14" s="57"/>
       <c r="H14" s="57"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="42"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="54"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="14" t="str">
@@ -1506,8 +1513,8 @@
       <c r="F15" s="57"/>
       <c r="G15" s="57"/>
       <c r="H15" s="57"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="42"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="54"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="14" t="str">
@@ -1533,8 +1540,8 @@
       <c r="F16" s="57"/>
       <c r="G16" s="57"/>
       <c r="H16" s="57"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="54"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="14" t="str">
@@ -1560,8 +1567,8 @@
       <c r="F17" s="57"/>
       <c r="G17" s="57"/>
       <c r="H17" s="57"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="42"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="54"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="14" t="str">
@@ -1587,8 +1594,8 @@
       <c r="F18" s="57"/>
       <c r="G18" s="57"/>
       <c r="H18" s="57"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="54"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="14" t="str">
@@ -1614,8 +1621,8 @@
       <c r="F19" s="57"/>
       <c r="G19" s="57"/>
       <c r="H19" s="57"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="54"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="14" t="str">
@@ -1641,8 +1648,8 @@
       <c r="F20" s="57"/>
       <c r="G20" s="57"/>
       <c r="H20" s="57"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="42"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="54"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
       <c r="M20" s="14" t="str">
@@ -1668,8 +1675,8 @@
       <c r="F21" s="57"/>
       <c r="G21" s="57"/>
       <c r="H21" s="57"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="42"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="54"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
       <c r="M21" s="14" t="str">
@@ -1695,8 +1702,8 @@
       <c r="F22" s="57"/>
       <c r="G22" s="57"/>
       <c r="H22" s="57"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="42"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="54"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="14" t="str">
@@ -1722,8 +1729,8 @@
       <c r="F23" s="57"/>
       <c r="G23" s="57"/>
       <c r="H23" s="57"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="42"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="54"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
       <c r="M23" s="14" t="str">
@@ -1749,8 +1756,8 @@
       <c r="F24" s="57"/>
       <c r="G24" s="57"/>
       <c r="H24" s="57"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="42"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="54"/>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
       <c r="M24" s="14" t="str">
@@ -1776,8 +1783,8 @@
       <c r="F25" s="57"/>
       <c r="G25" s="57"/>
       <c r="H25" s="57"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="42"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="54"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="14" t="str">
@@ -1803,8 +1810,8 @@
       <c r="F26" s="57"/>
       <c r="G26" s="57"/>
       <c r="H26" s="57"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="42"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="54"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="14" t="str">
@@ -1830,8 +1837,8 @@
       <c r="F27" s="58"/>
       <c r="G27" s="58"/>
       <c r="H27" s="58"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="55"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="60"/>
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
       <c r="M27" s="20" t="str">
@@ -1849,14 +1856,14 @@
       <c r="B28" s="21">
         <v>2.4</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
       <c r="I28" s="62"/>
       <c r="J28" s="63"/>
       <c r="K28" s="22"/>
@@ -1876,14 +1883,14 @@
       <c r="B29" s="21">
         <v>4.3</v>
       </c>
-      <c r="C29" s="59" t="s">
+      <c r="C29" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
       <c r="I29" s="62"/>
       <c r="J29" s="63"/>
       <c r="K29" s="22"/>
@@ -1927,16 +1934,16 @@
       <c r="B31" s="24">
         <v>6.3</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="52"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="72"/>
       <c r="K31" s="25"/>
       <c r="L31" s="25"/>
       <c r="M31" s="26" t="str">
@@ -1962,8 +1969,8 @@
       <c r="F32" s="58"/>
       <c r="G32" s="58"/>
       <c r="H32" s="58"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="55"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="60"/>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
       <c r="M32" s="20" t="str">
@@ -1981,14 +1988,14 @@
       <c r="B33" s="21">
         <v>7.4</v>
       </c>
-      <c r="C33" s="59" t="s">
+      <c r="C33" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
       <c r="I33" s="62"/>
       <c r="J33" s="63"/>
       <c r="K33" s="22"/>
@@ -2043,8 +2050,8 @@
       <c r="F35" s="58"/>
       <c r="G35" s="58"/>
       <c r="H35" s="58"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="55"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="60"/>
       <c r="K35" s="30"/>
       <c r="L35" s="30"/>
       <c r="M35" s="20" t="str">
@@ -2062,16 +2069,16 @@
       <c r="B36" s="31">
         <v>9.4</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="52"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="72"/>
       <c r="K36" s="32"/>
       <c r="L36" s="32"/>
       <c r="M36" s="26" t="str">
@@ -2097,8 +2104,8 @@
       <c r="F37" s="57"/>
       <c r="G37" s="57"/>
       <c r="H37" s="57"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="42"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="54"/>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
       <c r="M37" s="14" t="str">
@@ -2124,8 +2131,8 @@
       <c r="F38" s="57"/>
       <c r="G38" s="57"/>
       <c r="H38" s="57"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="42"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="54"/>
       <c r="K38" s="17"/>
       <c r="L38" s="17"/>
       <c r="M38" s="14" t="str">
@@ -2151,8 +2158,8 @@
       <c r="F39" s="57"/>
       <c r="G39" s="57"/>
       <c r="H39" s="57"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="42"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="54"/>
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
       <c r="M39" s="14" t="str">
@@ -2178,8 +2185,8 @@
       <c r="F40" s="57"/>
       <c r="G40" s="57"/>
       <c r="H40" s="57"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="42"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="54"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
       <c r="M40" s="14" t="str">
@@ -2205,8 +2212,8 @@
       <c r="F41" s="57"/>
       <c r="G41" s="57"/>
       <c r="H41" s="57"/>
-      <c r="I41" s="41"/>
-      <c r="J41" s="42"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="54"/>
       <c r="K41" s="17"/>
       <c r="L41" s="17"/>
       <c r="M41" s="14" t="str">
@@ -2232,8 +2239,8 @@
       <c r="F42" s="58"/>
       <c r="G42" s="58"/>
       <c r="H42" s="58"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="55"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="60"/>
       <c r="K42" s="30"/>
       <c r="L42" s="30"/>
       <c r="M42" s="20" t="str">
@@ -2251,16 +2258,16 @@
       <c r="B43" s="24">
         <v>10.1</v>
       </c>
-      <c r="C43" s="56" t="s">
+      <c r="C43" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="52"/>
+      <c r="D43" s="70"/>
+      <c r="E43" s="70"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="72"/>
       <c r="K43" s="32"/>
       <c r="L43" s="32"/>
       <c r="M43" s="14" t="str">
@@ -2286,8 +2293,8 @@
       <c r="F44" s="58"/>
       <c r="G44" s="58"/>
       <c r="H44" s="58"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="55"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="60"/>
       <c r="K44" s="30"/>
       <c r="L44" s="30"/>
       <c r="M44" s="14" t="str">
@@ -2305,16 +2312,16 @@
       <c r="B45" s="21">
         <v>11.5</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="73"/>
+      <c r="J45" s="74"/>
       <c r="K45" s="34"/>
       <c r="L45" s="35">
         <v>1</v>
@@ -2334,16 +2341,16 @@
       <c r="B46" s="21">
         <v>12.3</v>
       </c>
-      <c r="C46" s="59" t="s">
+      <c r="C46" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="59"/>
-      <c r="I46" s="60"/>
-      <c r="J46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="73"/>
+      <c r="J46" s="74"/>
       <c r="K46" s="35">
         <v>9</v>
       </c>
@@ -2363,16 +2370,16 @@
       <c r="B47" s="24">
         <v>13.1</v>
       </c>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="52"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="71"/>
+      <c r="J47" s="72"/>
       <c r="K47" s="32"/>
       <c r="L47" s="32"/>
       <c r="M47" s="14" t="str">
@@ -2398,8 +2405,8 @@
       <c r="F48" s="57"/>
       <c r="G48" s="57"/>
       <c r="H48" s="57"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="42"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="54"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
       <c r="M48" s="14" t="str">
@@ -2425,8 +2432,8 @@
       <c r="F49" s="57"/>
       <c r="G49" s="57"/>
       <c r="H49" s="57"/>
-      <c r="I49" s="41"/>
-      <c r="J49" s="42"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="54"/>
       <c r="K49" s="36">
         <v>9</v>
       </c>
@@ -2446,16 +2453,16 @@
       <c r="B50" s="12">
         <v>13.6</v>
       </c>
-      <c r="C50" s="40" t="s">
+      <c r="C50" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="40"/>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="42"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="52"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="54"/>
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
       <c r="M50" s="14" t="str">
@@ -2473,16 +2480,16 @@
       <c r="B51" s="12">
         <v>13.8</v>
       </c>
-      <c r="C51" s="40" t="s">
+      <c r="C51" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="42"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="53"/>
+      <c r="J51" s="54"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17"/>
       <c r="M51" s="14" t="str">
@@ -2500,16 +2507,16 @@
       <c r="B52" s="18">
         <v>13.9</v>
       </c>
-      <c r="C52" s="53" t="s">
+      <c r="C52" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="54"/>
-      <c r="J52" s="55"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="82"/>
+      <c r="I52" s="59"/>
+      <c r="J52" s="60"/>
       <c r="K52" s="30"/>
       <c r="L52" s="30"/>
       <c r="M52" s="14" t="str">
@@ -2527,16 +2534,16 @@
       <c r="B53" s="24">
         <v>14.8</v>
       </c>
-      <c r="C53" s="50" t="s">
+      <c r="C53" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="50"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="50"/>
-      <c r="H53" s="50"/>
-      <c r="I53" s="51"/>
-      <c r="J53" s="52"/>
+      <c r="D53" s="81"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="81"/>
+      <c r="G53" s="81"/>
+      <c r="H53" s="81"/>
+      <c r="I53" s="71"/>
+      <c r="J53" s="72"/>
       <c r="K53" s="32"/>
       <c r="L53" s="32"/>
       <c r="M53" s="14" t="str">
@@ -2554,16 +2561,16 @@
       <c r="B54" s="12">
         <v>14.9</v>
       </c>
-      <c r="C54" s="40" t="s">
+      <c r="C54" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="41"/>
-      <c r="J54" s="42"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="52"/>
+      <c r="H54" s="52"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="54"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
       <c r="M54" s="14" t="str">
@@ -2581,16 +2588,16 @@
       <c r="B55" s="37">
         <v>14.1</v>
       </c>
-      <c r="C55" s="40" t="s">
+      <c r="C55" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="41"/>
-      <c r="J55" s="42"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="52"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="54"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
       <c r="M55" s="14" t="str">
@@ -2608,16 +2615,16 @@
       <c r="B56" s="12">
         <v>14.11</v>
       </c>
-      <c r="C56" s="40" t="s">
+      <c r="C56" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="42"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="54"/>
       <c r="K56" s="17"/>
       <c r="L56" s="17"/>
       <c r="M56" s="14" t="str">
@@ -2648,23 +2655,23 @@
     </row>
     <row r="58" spans="1:15" s="2" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
-      <c r="B58" s="43" t="s">
+      <c r="B58" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="44"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="46"/>
+      <c r="C58" s="76"/>
+      <c r="D58" s="76"/>
+      <c r="E58" s="76"/>
+      <c r="F58" s="76"/>
+      <c r="G58" s="76"/>
+      <c r="H58" s="77"/>
+      <c r="I58" s="78"/>
+      <c r="J58" s="78"/>
       <c r="K58" s="38"/>
-      <c r="L58" s="47" t="str">
+      <c r="L58" s="79" t="str">
         <f>IF(Q67&lt;Q66,"",IF(Q67&gt;Q66,"Fail","Pass"))</f>
         <v/>
       </c>
-      <c r="M58" s="48"/>
+      <c r="M58" s="80"/>
       <c r="N58" s="1"/>
     </row>
     <row r="59" spans="1:15" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3236,91 +3243,6 @@
     </row>
   </sheetData>
   <mergeCells count="109">
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="C44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="C45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="C42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="C43:H43"/>
-    <mergeCell ref="I43:J43"/>
     <mergeCell ref="C56:H56"/>
     <mergeCell ref="I56:J56"/>
     <mergeCell ref="B58:H58"/>
@@ -3345,6 +3267,91 @@
     <mergeCell ref="I48:J48"/>
     <mergeCell ref="C49:H49"/>
     <mergeCell ref="I49:J49"/>
+    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="C45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="L58 M59">
     <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
@@ -3372,4 +3379,35 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3C07D2-A121-4F19-87C7-F819B1E58E49}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>